<commit_message>
add more detail on estimated gas costs, change smart contract name, add programming environment detail
</commit_message>
<xml_diff>
--- a/presentation/experiment environment table.xlsx
+++ b/presentation/experiment environment table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ardhito\Academic\TU-Berlin\1st Semester\Cloud Prototyping\Experiment\cp_ws_1920\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ardhito\Academic\TU-Berlin\1st Semester\Cloud Prototyping\Experiment\cp_ws_1920\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09C201A5-1487-4E32-AB8E-CC7CC60E58C8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B1B3B2-86F7-4501-8CC1-AA87761B0851}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{499C2736-B813-4218-B8AB-3D5AB18C48DB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Workload</t>
   </si>
@@ -57,12 +57,6 @@
     <t>Smart Contract</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>simple.json</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
@@ -97,13 +91,31 @@
   </si>
   <si>
     <t>2, 5, 15, 20</t>
+  </si>
+  <si>
+    <t>File Used</t>
+  </si>
+  <si>
+    <t>Submit contract: 411096 gas</t>
+  </si>
+  <si>
+    <t>open: 23219 gas ; query: 25819 gas ; transfer: 30688 gas</t>
+  </si>
+  <si>
+    <t>Programming environment</t>
+  </si>
+  <si>
+    <t>simple.sol</t>
+  </si>
+  <si>
+    <t>solidity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +129,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -139,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -162,29 +180,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,30 +567,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A51EA9-F3DA-42CA-8A41-4D1F6D0D9A21}">
-  <dimension ref="B3:D17"/>
+  <dimension ref="B3:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1"/>
-    <col min="2" max="2" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="11.5546875" style="2"/>
+    <col min="2" max="2" width="16.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -531,8 +598,8 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -540,8 +607,8 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -549,88 +616,107 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" ht="28.8" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="7">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="3">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="4"/>
+      <c r="D18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
change the details for smart contract, workload, system under test
</commit_message>
<xml_diff>
--- a/presentation/experiment environment table.xlsx
+++ b/presentation/experiment environment table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ardhito\Academic\TU-Berlin\1st Semester\Cloud Prototyping\Experiment\cp_ws_1920\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B1B3B2-86F7-4501-8CC1-AA87761B0851}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE466E22-48DC-4610-962D-C78DAE75EEF8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{499C2736-B813-4218-B8AB-3D5AB18C48DB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Workload</t>
   </si>
@@ -42,36 +42,21 @@
     <t>Hyperledger Caliper</t>
   </si>
   <si>
-    <t>Distance</t>
-  </si>
-  <si>
-    <t>Local machine - Google Cloud Platform (europe-west1-b server)</t>
-  </si>
-  <si>
     <t>Transaction</t>
   </si>
   <si>
-    <t>200 tps</t>
-  </si>
-  <si>
     <t>Smart Contract</t>
   </si>
   <si>
     <t>Function</t>
   </si>
   <si>
-    <t>open, query, transfer</t>
-  </si>
-  <si>
     <t>Estimated Gas Cost</t>
   </si>
   <si>
     <t>System Under Test Configuration</t>
   </si>
   <si>
-    <t>1vCPU ; 3.75GB memory ; Intel Haswell</t>
-  </si>
-  <si>
     <t>Machine Type</t>
   </si>
   <si>
@@ -81,15 +66,9 @@
     <t>Number of Nodes</t>
   </si>
   <si>
-    <t>Gas Limit</t>
-  </si>
-  <si>
     <t>4, 6, 8, 10, 12, 14, 16, 18, 20, 40, 100</t>
   </si>
   <si>
-    <t>Block Interval</t>
-  </si>
-  <si>
     <t>2, 5, 15, 20</t>
   </si>
   <si>
@@ -99,16 +78,42 @@
     <t>Submit contract: 411096 gas</t>
   </si>
   <si>
-    <t>open: 23219 gas ; query: 25819 gas ; transfer: 30688 gas</t>
-  </si>
-  <si>
-    <t>Programming environment</t>
-  </si>
-  <si>
     <t>simple.sol</t>
   </si>
   <si>
     <t>solidity</t>
+  </si>
+  <si>
+    <t>open, transfer</t>
+  </si>
+  <si>
+    <t>open: 23219 gas ; transfer: 30688 gas</t>
+  </si>
+  <si>
+    <t>Programming language</t>
+  </si>
+  <si>
+    <t>Gas Limit 
+(in millions)</t>
+  </si>
+  <si>
+    <t>Block Interval 
+(seconds)</t>
+  </si>
+  <si>
+    <t>1 bootnode, 2 sealer nodes</t>
+  </si>
+  <si>
+    <t>Machine type</t>
+  </si>
+  <si>
+    <t>Macbook pro 13' 2015</t>
+  </si>
+  <si>
+    <t>transaction rate: 100tps</t>
+  </si>
+  <si>
+    <t>Region: europe-west1-b (Belgium); 1vCPU ; 3.75GB memory ; Intel Haswell</t>
   </si>
 </sst>
 </file>
@@ -223,9 +228,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -251,6 +253,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,153 +575,157 @@
   <dimension ref="B3:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="2"/>
-    <col min="2" max="2" width="16.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.109375" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="16.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="C12" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="2:6" ht="28.8" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="2:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="7">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add more detail on transaction, add detail on gas limit & block interval
</commit_message>
<xml_diff>
--- a/presentation/experiment environment table.xlsx
+++ b/presentation/experiment environment table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ardhito\Academic\TU-Berlin\1st Semester\Cloud Prototyping\Experiment\cp_ws_1920\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE466E22-48DC-4610-962D-C78DAE75EEF8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0A220C-B018-438E-8C54-257CD0D0CDC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{499C2736-B813-4218-B8AB-3D5AB18C48DB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Workload</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Region: europe-west1-b (Belgium); 1vCPU ; 3.75GB memory ; Intel Haswell</t>
+  </si>
+  <si>
+    <t>20s block interval</t>
+  </si>
+  <si>
+    <t>100millions Gas Limit</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
   <dimension ref="B3:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +716,9 @@
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
@@ -719,7 +727,9 @@
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
add new details for block gas limit and block interval
</commit_message>
<xml_diff>
--- a/presentation/experiment environment table.xlsx
+++ b/presentation/experiment environment table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ardhito\Academic\TU-Berlin\1st Semester\Cloud Prototyping\Experiment\cp_ws_1920\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0A220C-B018-438E-8C54-257CD0D0CDC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5D1AC6-CB6D-4A0A-8356-3E5896CAF0FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{499C2736-B813-4218-B8AB-3D5AB18C48DB}"/>
+    <workbookView minimized="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{499C2736-B813-4218-B8AB-3D5AB18C48DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
     <t>20s block interval</t>
   </si>
   <si>
-    <t>100millions Gas Limit</t>
+    <t>100million Gas Limit</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="B3:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>